<commit_message>
make 3 apps & adjust each DB
</commit_message>
<xml_diff>
--- a/DB_Scheme.xlsx
+++ b/DB_Scheme.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koesnam/Desktop/myApps/3DPrintingPlatform/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCF8F72-523A-944F-8481-3BE5212BB032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C568180-120B-FC40-B90F-3E8BA1623314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{8863869B-68AD-5A41-8A35-1A81322B5D17}"/>
+    <workbookView xWindow="19500" yWindow="740" windowWidth="10740" windowHeight="18900" xr2:uid="{8863869B-68AD-5A41-8A35-1A81322B5D17}"/>
   </bookViews>
   <sheets>
     <sheet name="정리본" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="96">
   <si>
     <t>구매자</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -411,6 +411,14 @@
   </si>
   <si>
     <t>판매자&lt;-&gt;제조장비</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>견적ID : uuid</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>입찰ID : uuid</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -900,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B86B513-BC45-2847-8AF9-D2CE8E39BB24}">
   <dimension ref="B5:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -1015,7 +1023,7 @@
         <v>77</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="2:7">
@@ -1026,7 +1034,7 @@
         <v>73</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>84</v>
@@ -1043,7 +1051,7 @@
         <v>78</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="3:7">

</xml_diff>